<commit_message>
Added classification for 200R steel datasets.
</commit_message>
<xml_diff>
--- a/IEDC_LookupTable_fill/classification_definition_data.xlsx
+++ b/IEDC_LookupTable_fill/classification_definition_data.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="105">
   <si>
     <t>id</t>
   </si>
@@ -290,6 +290,45 @@
   </si>
   <si>
     <t>List of time intervals for age cohorts</t>
+  </si>
+  <si>
+    <t>steel_cycle_200R_processes</t>
+  </si>
+  <si>
+    <t>List of processes for steel cycle MFA DOI 10.1016/j.resconrec.2012.11.008</t>
+  </si>
+  <si>
+    <t>process_id</t>
+  </si>
+  <si>
+    <t>process_name</t>
+  </si>
+  <si>
+    <t>process_code</t>
+  </si>
+  <si>
+    <t>process_type</t>
+  </si>
+  <si>
+    <t>comment</t>
+  </si>
+  <si>
+    <t>color</t>
+  </si>
+  <si>
+    <t>angle</t>
+  </si>
+  <si>
+    <t>width</t>
+  </si>
+  <si>
+    <t>height</t>
+  </si>
+  <si>
+    <t>xPos</t>
+  </si>
+  <si>
+    <t>yPos</t>
   </si>
 </sst>
 </file>
@@ -663,12 +702,12 @@
   <dimension ref="A1:AA24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J8" sqref="J8"/>
+      <selection activeCell="N18" sqref="N18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="21" customWidth="1"/>
+    <col min="2" max="2" width="24.77734375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="19.33203125" customWidth="1"/>
     <col min="4" max="4" width="18.109375" customWidth="1"/>
     <col min="5" max="5" width="17.5546875" customWidth="1"/>
@@ -1469,78 +1508,104 @@
       <c r="AA16" s="5"/>
     </row>
     <row r="17" spans="1:27" x14ac:dyDescent="0.3">
-      <c r="A17" s="3"/>
-      <c r="B17" s="5"/>
-      <c r="C17" s="5"/>
-      <c r="D17" s="5"/>
-      <c r="E17" s="5"/>
-      <c r="F17" s="5"/>
+      <c r="A17" s="6">
+        <v>15</v>
+      </c>
+      <c r="B17" t="s">
+        <v>86</v>
+      </c>
+      <c r="C17">
+        <v>0</v>
+      </c>
+      <c r="D17" t="s">
+        <v>87</v>
+      </c>
+      <c r="E17" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="F17" s="5" t="s">
+        <v>37</v>
+      </c>
       <c r="G17" s="5"/>
-      <c r="H17" s="5"/>
-      <c r="I17" s="5"/>
-      <c r="J17" s="5"/>
-      <c r="K17" s="5"/>
-      <c r="L17" s="5"/>
-      <c r="M17" s="5"/>
-      <c r="N17" s="5"/>
-      <c r="O17" s="5"/>
-      <c r="P17" s="5"/>
-      <c r="Q17" s="5"/>
-      <c r="R17" s="5"/>
-      <c r="S17" s="5"/>
-      <c r="T17" s="5"/>
-      <c r="U17" s="5"/>
-      <c r="V17" s="5"/>
-      <c r="W17" s="5"/>
+      <c r="H17" s="5" t="s">
+        <v>30</v>
+      </c>
       <c r="X17" s="5"/>
       <c r="Y17" s="5"/>
       <c r="Z17" s="5"/>
       <c r="AA17" s="5"/>
     </row>
     <row r="18" spans="1:27" x14ac:dyDescent="0.3">
-      <c r="A18" s="3"/>
-      <c r="B18" s="5"/>
-      <c r="C18" s="5"/>
-      <c r="D18" s="5"/>
-      <c r="E18" s="5"/>
-      <c r="F18" s="5"/>
+      <c r="A18" s="3">
+        <v>16</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="C18" s="5">
+        <v>7</v>
+      </c>
+      <c r="D18" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="E18" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="F18" s="5" t="s">
+        <v>37</v>
+      </c>
       <c r="G18" s="5"/>
-      <c r="H18" s="5"/>
+      <c r="H18" s="5" t="s">
+        <v>30</v>
+      </c>
       <c r="I18" s="5"/>
       <c r="J18" s="5"/>
       <c r="K18" s="5"/>
       <c r="L18" s="5"/>
-      <c r="M18" s="5"/>
-      <c r="N18" s="5"/>
-      <c r="O18" s="5"/>
-      <c r="P18" s="5"/>
-      <c r="Q18" s="5"/>
-      <c r="R18" s="5"/>
-      <c r="S18" s="5"/>
-      <c r="T18" s="5"/>
-      <c r="U18" s="5"/>
-      <c r="V18" s="5"/>
-      <c r="W18" s="5"/>
+      <c r="M18" t="s">
+        <v>95</v>
+      </c>
+      <c r="N18" t="s">
+        <v>94</v>
+      </c>
+      <c r="O18" t="s">
+        <v>96</v>
+      </c>
+      <c r="P18" t="s">
+        <v>97</v>
+      </c>
+      <c r="Q18" t="s">
+        <v>98</v>
+      </c>
+      <c r="R18" t="s">
+        <v>99</v>
+      </c>
+      <c r="S18" t="s">
+        <v>100</v>
+      </c>
+      <c r="T18" t="s">
+        <v>101</v>
+      </c>
+      <c r="U18" t="s">
+        <v>102</v>
+      </c>
+      <c r="V18" t="s">
+        <v>103</v>
+      </c>
+      <c r="W18" t="s">
+        <v>104</v>
+      </c>
       <c r="X18" s="5"/>
       <c r="Y18" s="5"/>
       <c r="Z18" s="5"/>
       <c r="AA18" s="5"/>
     </row>
     <row r="19" spans="1:27" x14ac:dyDescent="0.3">
-      <c r="A19" s="3"/>
-      <c r="B19" s="5"/>
-      <c r="C19" s="5"/>
-      <c r="D19" s="5"/>
-      <c r="E19" s="5"/>
-      <c r="F19" s="5"/>
-      <c r="G19" s="5"/>
-      <c r="H19" s="5"/>
       <c r="I19" s="5"/>
       <c r="J19" s="5"/>
       <c r="K19" s="5"/>
       <c r="L19" s="5"/>
       <c r="M19" s="5"/>
-      <c r="N19" s="5"/>
       <c r="O19" s="5"/>
       <c r="P19" s="5"/>
       <c r="Q19" s="5"/>

</xml_diff>